<commit_message>
chore(stat): replace '降级为市' with '降为县级市'
</commit_message>
<xml_diff>
--- a/data/statistics/县级市.xlsx
+++ b/data/statistics/县级市.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asudy/Library/Mobile Documents/com~apple~CloudDocs/Education/College-Edu/4大二下/深度科研/频次统计/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asudy/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEE79D5-E178-A341-ACF7-2A6CC1D43E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5F3154-A354-E645-9D49-D6E83D3DB746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7780" yWindow="500" windowWidth="24560" windowHeight="13440" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="按省份分" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>撤县设市</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -311,10 +311,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>降级</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>总计</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -322,7 +318,7 @@
     <t>总计</t>
   </si>
   <si>
-    <t>降级为市</t>
+    <t>降为县级市</t>
   </si>
 </sst>
 </file>
@@ -1697,13 +1693,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF6"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="V28" sqref="V28"/>
+    <sheetView zoomScale="185" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="21" x14ac:dyDescent="0.25">
@@ -2035,7 +2032,7 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J5" s="1">
         <v>1</v>
@@ -2043,7 +2040,7 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" s="1">
         <f>SUM([1]Sheet1!D3:D44)</f>
@@ -2179,7 +2176,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2197,10 +2194,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>